<commit_message>
second On branch main Your branch is up to date with 'Comparednet/main'.
Changes to be committed:
	modified:   README.md
	modified:   result/compared_result.xlsx
</commit_message>
<xml_diff>
--- a/result/compared_result.xlsx
+++ b/result/compared_result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\云计算大作业\CompareNet_FakeNewsDetection-master\result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7A28FD1-02D3-40CB-8737-C5B07CA247AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B6450E0-6C9C-4AB7-8EE9-655C3F4E99C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -113,9 +113,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -407,7 +413,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -416,123 +422,123 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="1"/>
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="4"/>
+      <c r="D2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2">
-        <v>55.34</v>
-      </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2">
-        <v>55.17</v>
-      </c>
-      <c r="E3" s="2">
-        <v>55.34</v>
-      </c>
-      <c r="F3" s="2">
-        <v>55.37</v>
+      <c r="B3" s="4">
+        <v>65.34</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4">
+        <v>65.17</v>
+      </c>
+      <c r="E3" s="4">
+        <v>65.34</v>
+      </c>
+      <c r="F3" s="4">
+        <v>65.37</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="2">
-        <v>53.85</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2">
-        <v>53.59</v>
-      </c>
-      <c r="E4" s="2">
-        <v>53.85</v>
-      </c>
-      <c r="F4" s="2">
-        <v>53.78</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="B4" s="4">
+        <v>73.849999999999994</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4">
+        <v>73.59</v>
+      </c>
+      <c r="E4" s="4">
+        <v>73.849999999999994</v>
+      </c>
+      <c r="F4" s="4">
+        <v>73.78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2">
-        <v>58.34</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2">
-        <v>57.65</v>
-      </c>
-      <c r="E5" s="2">
-        <v>58.33</v>
-      </c>
-      <c r="F5" s="2">
-        <v>58.31</v>
+      <c r="B5" s="4">
+        <v>78.34</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4">
+        <v>77.650000000000006</v>
+      </c>
+      <c r="E5" s="4">
+        <v>78.33</v>
+      </c>
+      <c r="F5" s="4">
+        <v>78.31</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="2">
-        <v>60.78</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2">
-        <v>61.49</v>
-      </c>
-      <c r="E6" s="2">
-        <v>60.78</v>
-      </c>
-      <c r="F6" s="2">
-        <v>60.76</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="B6" s="4">
+        <v>80.78</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4">
+        <v>81.489999999999995</v>
+      </c>
+      <c r="E6" s="4">
+        <v>80.78</v>
+      </c>
+      <c r="F6" s="4">
+        <v>80.760000000000005</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="3">
-        <v>62.63</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3">
-        <v>63.75</v>
-      </c>
-      <c r="E7" s="3">
-        <v>62.63</v>
-      </c>
-      <c r="F7" s="3">
-        <v>62.65</v>
+      <c r="B7" s="5">
+        <v>82.63</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5">
+        <v>83.75</v>
+      </c>
+      <c r="E7" s="5">
+        <v>82.63</v>
+      </c>
+      <c r="F7" s="5">
+        <v>82.65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>